<commit_message>
tried to make flow chart
</commit_message>
<xml_diff>
--- a/Data/Raw/Flow Steps.xlsx
+++ b/Data/Raw/Flow Steps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\pet-inflation\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926D0FFD-FC8F-4925-916F-076AA13EB488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5FE187-7DEC-4656-BF3F-C2D4C2C19A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Step</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -187,6 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,18 +471,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="31.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,8 +502,11 @@
       <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -517,8 +525,11 @@
       <c r="F2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="G2" s="3">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -537,8 +548,11 @@
       <c r="F3" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="G3" s="3">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -557,8 +571,11 @@
       <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+      <c r="G4" s="3">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -577,8 +594,11 @@
       <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="403.2" x14ac:dyDescent="0.3">
+      <c r="G5" s="3">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -597,8 +617,11 @@
       <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="G6" s="3">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -617,8 +640,11 @@
       <c r="F7" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="G7" s="3">
+        <v>45809</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -637,8 +663,11 @@
       <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="288" x14ac:dyDescent="0.3">
+      <c r="G8" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -657,8 +686,11 @@
       <c r="F9" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="G9" s="3">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -677,8 +709,11 @@
       <c r="F10" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="G10" s="3">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -696,6 +731,9 @@
       </c>
       <c r="F11" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="G11" s="3">
+        <v>45931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>